<commit_message>
Github Auto Build at 2024-05-11 10:09
</commit_message>
<xml_diff>
--- a/resource/cost.xlsx
+++ b/resource/cost.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2158"/>
+  <dimension ref="A1:B2159"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22015,6 +22015,16 @@
         <v>0.0008</v>
       </c>
     </row>
+    <row r="2159">
+      <c r="A2159" t="inlineStr">
+        <is>
+          <t>2024-05-11 10:09:36</t>
+        </is>
+      </c>
+      <c r="B2159" t="n">
+        <v>0.0014</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Github Auto Build at 2024-05-11 11:29
</commit_message>
<xml_diff>
--- a/resource/cost.xlsx
+++ b/resource/cost.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,6 +475,16 @@
         <v>0.0008</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2024-05-11 11:29:48</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.0004</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Github Auto Build at 2024-05-11 21:27
</commit_message>
<xml_diff>
--- a/resource/cost.xlsx
+++ b/resource/cost.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,6 +485,36 @@
         <v>0.0004</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2024-05-11 21:26:21</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.0002</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2024-05-11 21:26:59</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2024-05-11 21:27:23</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.0006000000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>